<commit_message>
excel sort with date
</commit_message>
<xml_diff>
--- a/website/static/excel/AssignedMatches.xlsx
+++ b/website/static/excel/AssignedMatches.xlsx
@@ -37,54 +37,141 @@
     <t>Date</t>
   </si>
   <si>
+    <t>ZEYTINBURNUSPOR</t>
+  </si>
+  <si>
+    <t>KARACAAHMETSPOR</t>
+  </si>
+  <si>
+    <t>3.GRUP</t>
+  </si>
+  <si>
+    <t>Kartal 75 Sahasi</t>
+  </si>
+  <si>
+    <t>SUNDAY</t>
+  </si>
+  <si>
+    <t>SLOT5</t>
+  </si>
+  <si>
+    <t>YILDIZSPOR</t>
+  </si>
+  <si>
+    <t>SULTANBEYLISPOR</t>
+  </si>
+  <si>
+    <t>SATURDAY</t>
+  </si>
+  <si>
+    <t>SLOT2</t>
+  </si>
+  <si>
+    <t>SISLISPOR</t>
+  </si>
+  <si>
+    <t>EMINONUSPOR</t>
+  </si>
+  <si>
+    <t>SLOT3</t>
+  </si>
+  <si>
+    <t>YENI UFUKSPOR</t>
+  </si>
+  <si>
+    <t>SILE YILDIZ SPOR</t>
+  </si>
+  <si>
+    <t>1.GRUP</t>
+  </si>
+  <si>
+    <t>Yahya Kemal Sahasi</t>
+  </si>
+  <si>
+    <t>THURSDAY</t>
+  </si>
+  <si>
+    <t>NISANTASISPOR</t>
+  </si>
+  <si>
+    <t>ISTANBUL ANADOLU FUTBOL YATIRIMLARI</t>
+  </si>
+  <si>
+    <t>SLOT4</t>
+  </si>
+  <si>
+    <t>ESENYURTSPOR</t>
+  </si>
+  <si>
+    <t>SILIVRISPOR</t>
+  </si>
+  <si>
+    <t>2.GRUP</t>
+  </si>
+  <si>
+    <t>Dudullu Sahasi</t>
+  </si>
+  <si>
+    <t>WEDNESDAY</t>
+  </si>
+  <si>
+    <t>SARIYER YENIMAHALLESPOR</t>
+  </si>
+  <si>
+    <t>ALIBEYKOYSPOR</t>
+  </si>
+  <si>
+    <t>Silivri Sahasi</t>
+  </si>
+  <si>
+    <t>TUESDAY</t>
+  </si>
+  <si>
+    <t>CAFERAGASPOR</t>
+  </si>
+  <si>
+    <t>YENIKOYSPOR</t>
+  </si>
+  <si>
+    <t>SLOT1</t>
+  </si>
+  <si>
+    <t>BEYOGLUSPOR</t>
+  </si>
+  <si>
+    <t>CIBALISPOR</t>
+  </si>
+  <si>
+    <t>CADDEBOSTANSPOR</t>
+  </si>
+  <si>
+    <t>SULTANAHMETSPOR</t>
+  </si>
+  <si>
     <t>MALTEPESPOR</t>
   </si>
   <si>
     <t>KARTAL SPORTIF FAALIYETLERI</t>
   </si>
   <si>
-    <t>1.GRUP</t>
-  </si>
-  <si>
     <t>Beykoz Sahasi</t>
   </si>
   <si>
     <t>MONDAY</t>
   </si>
   <si>
-    <t>SLOT1</t>
-  </si>
-  <si>
     <t>BEYKOZ ISHAKLI SPOR FAALIYETLERI</t>
   </si>
   <si>
     <t>ISTANBUL BEYLIKDUZUSPOR</t>
   </si>
   <si>
-    <t>Silivri Sahasi</t>
-  </si>
-  <si>
-    <t>SARIYER YENIMAHALLESPOR</t>
-  </si>
-  <si>
-    <t>ALIBEYKOYSPOR</t>
-  </si>
-  <si>
-    <t>TUESDAY</t>
-  </si>
-  <si>
-    <t>SLOT2</t>
-  </si>
-  <si>
     <t>HALICSPOR</t>
   </si>
   <si>
     <t>VEFASPOR</t>
   </si>
   <si>
-    <t>Dudullu Sahasi</t>
-  </si>
-  <si>
     <t>INKILAP FUTBOL SPOR KULUBU</t>
   </si>
   <si>
@@ -94,75 +181,36 @@
     <t>Seyrantepe Sahasi</t>
   </si>
   <si>
-    <t>YENI UFUKSPOR</t>
-  </si>
-  <si>
-    <t>SILE YILDIZ SPOR</t>
-  </si>
-  <si>
-    <t>Yahya Kemal Sahasi</t>
-  </si>
-  <si>
-    <t>THURSDAY</t>
-  </si>
-  <si>
     <t>BEYLERBEYI 1911 FUTBOL KULUBU</t>
   </si>
   <si>
     <t>KUCUKCEKMECE SPORTIF FAALIYETLERI</t>
   </si>
   <si>
-    <t>NISANTASISPOR</t>
-  </si>
-  <si>
-    <t>ISTANBUL ANADOLU FUTBOL YATIRIMLARI</t>
-  </si>
-  <si>
-    <t>SLOT4</t>
-  </si>
-  <si>
     <t>FATIH KARAGUMRUK SPOR</t>
   </si>
   <si>
     <t>BAHCESEHIRSPOR</t>
   </si>
   <si>
-    <t>2.GRUP</t>
-  </si>
-  <si>
     <t>ABBASAGASPOR</t>
   </si>
   <si>
     <t>EYUPSULTANSPOR</t>
   </si>
   <si>
-    <t>SLOT3</t>
-  </si>
-  <si>
     <t>ESENLERSPOR</t>
   </si>
   <si>
     <t>KARTALSPOR</t>
   </si>
   <si>
-    <t>SLOT5</t>
-  </si>
-  <si>
     <t>FERIKOYSPOR</t>
   </si>
   <si>
     <t>KADIKOYSPOR</t>
   </si>
   <si>
-    <t>ESENYURTSPOR</t>
-  </si>
-  <si>
-    <t>SILIVRISPOR</t>
-  </si>
-  <si>
-    <t>WEDNESDAY</t>
-  </si>
-  <si>
     <t>GUNGORENSPOR</t>
   </si>
   <si>
@@ -181,64 +229,16 @@
     <t>BAGCILARSPOR</t>
   </si>
   <si>
-    <t>Kartal 75 Sahasi</t>
-  </si>
-  <si>
     <t>FLORYASPOR</t>
   </si>
   <si>
     <t>KABATASSPOR</t>
   </si>
   <si>
-    <t>3.GRUP</t>
-  </si>
-  <si>
     <t>SERENCEBEYSPOR</t>
   </si>
   <si>
     <t>TUZLASPOR</t>
-  </si>
-  <si>
-    <t>ZEYTINBURNUSPOR</t>
-  </si>
-  <si>
-    <t>KARACAAHMETSPOR</t>
-  </si>
-  <si>
-    <t>SUNDAY</t>
-  </si>
-  <si>
-    <t>CAFERAGASPOR</t>
-  </si>
-  <si>
-    <t>YENIKOYSPOR</t>
-  </si>
-  <si>
-    <t>YILDIZSPOR</t>
-  </si>
-  <si>
-    <t>SULTANBEYLISPOR</t>
-  </si>
-  <si>
-    <t>SATURDAY</t>
-  </si>
-  <si>
-    <t>BEYOGLUSPOR</t>
-  </si>
-  <si>
-    <t>CIBALISPOR</t>
-  </si>
-  <si>
-    <t>SISLISPOR</t>
-  </si>
-  <si>
-    <t>EMINONUSPOR</t>
-  </si>
-  <si>
-    <t>CADDEBOSTANSPOR</t>
-  </si>
-  <si>
-    <t>SULTANAHMETSPOR</t>
   </si>
 </sst>
 </file>
@@ -776,7 +776,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -796,7 +796,7 @@
         <v>12</v>
       </c>
       <c r="G2" s="7">
-        <v>45264</v>
+        <v>45270</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
@@ -810,39 +810,39 @@
         <v>9</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G3" s="7">
-        <v>45264</v>
+        <v>45269</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G4" s="7">
-        <v>45265</v>
+        <v>45269</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
@@ -853,177 +853,177 @@
         <v>21</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G5" s="7">
-        <v>45264</v>
+        <v>45267</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="F6" s="4" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="G6" s="7">
-        <v>45264</v>
+        <v>45267</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G7" s="7">
-        <v>45267</v>
+        <v>45266</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G8" s="7">
-        <v>45264</v>
+        <v>45265</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="4" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="G9" s="7">
-        <v>45267</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
+        <v>45265</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="4" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="F10" s="4" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="G10" s="7">
-        <v>45264</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+        <v>45265</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
       <c r="A11" s="4" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="7">
+        <v>45265</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
+      <c r="A12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G11" s="7">
-        <v>45264</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>43</v>
       </c>
       <c r="G12" s="7">
         <v>45264</v>
@@ -1031,22 +1031,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="4" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="G13" s="7">
         <v>45264</v>
@@ -1054,45 +1054,45 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="4" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="F14" s="4" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="G14" s="7">
-        <v>45266</v>
+        <v>45264</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="G15" s="7">
         <v>45264</v>
@@ -1100,45 +1100,45 @@
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="4" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="G16" s="7">
         <v>45264</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
       <c r="A17" s="4" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G17" s="7">
         <v>45264</v>
@@ -1146,22 +1146,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="4" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="G18" s="7">
         <v>45264</v>
@@ -1169,22 +1169,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="G19" s="7">
         <v>45264</v>
@@ -1192,71 +1192,71 @@
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="G20" s="7">
-        <v>45270</v>
+        <v>45264</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>12</v>
       </c>
       <c r="G21" s="7">
-        <v>45265</v>
+        <v>45264</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G22" s="7">
-        <v>45269</v>
+        <v>45264</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
@@ -1267,19 +1267,19 @@
         <v>70</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="G23" s="7">
-        <v>45265</v>
+        <v>45264</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
@@ -1290,22 +1290,22 @@
         <v>72</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="G24" s="7">
-        <v>45269</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="20.25">
+        <v>45264</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="4" t="s">
         <v>73</v>
       </c>
@@ -1313,19 +1313,19 @@
         <v>74</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="G25" s="7">
-        <v>45265</v>
+        <v>45264</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "excel sort with date"
This reverts commit 11471a83564fcd4069e9ad728a7f884aefda6871.
</commit_message>
<xml_diff>
--- a/website/static/excel/AssignedMatches.xlsx
+++ b/website/static/excel/AssignedMatches.xlsx
@@ -37,22 +37,181 @@
     <t>Date</t>
   </si>
   <si>
+    <t>MALTEPESPOR</t>
+  </si>
+  <si>
+    <t>KARTAL SPORTIF FAALIYETLERI</t>
+  </si>
+  <si>
+    <t>1.GRUP</t>
+  </si>
+  <si>
+    <t>Beykoz Sahasi</t>
+  </si>
+  <si>
+    <t>MONDAY</t>
+  </si>
+  <si>
+    <t>SLOT1</t>
+  </si>
+  <si>
+    <t>BEYKOZ ISHAKLI SPOR FAALIYETLERI</t>
+  </si>
+  <si>
+    <t>ISTANBUL BEYLIKDUZUSPOR</t>
+  </si>
+  <si>
+    <t>Silivri Sahasi</t>
+  </si>
+  <si>
+    <t>SARIYER YENIMAHALLESPOR</t>
+  </si>
+  <si>
+    <t>ALIBEYKOYSPOR</t>
+  </si>
+  <si>
+    <t>TUESDAY</t>
+  </si>
+  <si>
+    <t>SLOT2</t>
+  </si>
+  <si>
+    <t>HALICSPOR</t>
+  </si>
+  <si>
+    <t>VEFASPOR</t>
+  </si>
+  <si>
+    <t>Dudullu Sahasi</t>
+  </si>
+  <si>
+    <t>INKILAP FUTBOL SPOR KULUBU</t>
+  </si>
+  <si>
+    <t>BAYRAMPASA SPOR</t>
+  </si>
+  <si>
+    <t>Seyrantepe Sahasi</t>
+  </si>
+  <si>
+    <t>YENI UFUKSPOR</t>
+  </si>
+  <si>
+    <t>SILE YILDIZ SPOR</t>
+  </si>
+  <si>
+    <t>Yahya Kemal Sahasi</t>
+  </si>
+  <si>
+    <t>THURSDAY</t>
+  </si>
+  <si>
+    <t>BEYLERBEYI 1911 FUTBOL KULUBU</t>
+  </si>
+  <si>
+    <t>KUCUKCEKMECE SPORTIF FAALIYETLERI</t>
+  </si>
+  <si>
+    <t>NISANTASISPOR</t>
+  </si>
+  <si>
+    <t>ISTANBUL ANADOLU FUTBOL YATIRIMLARI</t>
+  </si>
+  <si>
+    <t>SLOT4</t>
+  </si>
+  <si>
+    <t>FATIH KARAGUMRUK SPOR</t>
+  </si>
+  <si>
+    <t>BAHCESEHIRSPOR</t>
+  </si>
+  <si>
+    <t>2.GRUP</t>
+  </si>
+  <si>
+    <t>ABBASAGASPOR</t>
+  </si>
+  <si>
+    <t>EYUPSULTANSPOR</t>
+  </si>
+  <si>
+    <t>SLOT3</t>
+  </si>
+  <si>
+    <t>ESENLERSPOR</t>
+  </si>
+  <si>
+    <t>KARTALSPOR</t>
+  </si>
+  <si>
+    <t>SLOT5</t>
+  </si>
+  <si>
+    <t>FERIKOYSPOR</t>
+  </si>
+  <si>
+    <t>KADIKOYSPOR</t>
+  </si>
+  <si>
+    <t>ESENYURTSPOR</t>
+  </si>
+  <si>
+    <t>SILIVRISPOR</t>
+  </si>
+  <si>
+    <t>WEDNESDAY</t>
+  </si>
+  <si>
+    <t>GUNGORENSPOR</t>
+  </si>
+  <si>
+    <t>BAKIRKOYSPOR</t>
+  </si>
+  <si>
+    <t>GAZIOSMANPASASPOR</t>
+  </si>
+  <si>
+    <t>SARIYERSPOR</t>
+  </si>
+  <si>
+    <t>TAKSIMSPOR</t>
+  </si>
+  <si>
+    <t>BAGCILARSPOR</t>
+  </si>
+  <si>
+    <t>Kartal 75 Sahasi</t>
+  </si>
+  <si>
+    <t>FLORYASPOR</t>
+  </si>
+  <si>
+    <t>KABATASSPOR</t>
+  </si>
+  <si>
+    <t>3.GRUP</t>
+  </si>
+  <si>
+    <t>SERENCEBEYSPOR</t>
+  </si>
+  <si>
+    <t>TUZLASPOR</t>
+  </si>
+  <si>
     <t>ZEYTINBURNUSPOR</t>
   </si>
   <si>
     <t>KARACAAHMETSPOR</t>
   </si>
   <si>
-    <t>3.GRUP</t>
-  </si>
-  <si>
-    <t>Kartal 75 Sahasi</t>
-  </si>
-  <si>
     <t>SUNDAY</t>
   </si>
   <si>
-    <t>SLOT5</t>
+    <t>CAFERAGASPOR</t>
+  </si>
+  <si>
+    <t>YENIKOYSPOR</t>
   </si>
   <si>
     <t>YILDIZSPOR</t>
@@ -64,7 +223,10 @@
     <t>SATURDAY</t>
   </si>
   <si>
-    <t>SLOT2</t>
+    <t>BEYOGLUSPOR</t>
+  </si>
+  <si>
+    <t>CIBALISPOR</t>
   </si>
   <si>
     <t>SISLISPOR</t>
@@ -73,172 +235,10 @@
     <t>EMINONUSPOR</t>
   </si>
   <si>
-    <t>SLOT3</t>
-  </si>
-  <si>
-    <t>YENI UFUKSPOR</t>
-  </si>
-  <si>
-    <t>SILE YILDIZ SPOR</t>
-  </si>
-  <si>
-    <t>1.GRUP</t>
-  </si>
-  <si>
-    <t>Yahya Kemal Sahasi</t>
-  </si>
-  <si>
-    <t>THURSDAY</t>
-  </si>
-  <si>
-    <t>NISANTASISPOR</t>
-  </si>
-  <si>
-    <t>ISTANBUL ANADOLU FUTBOL YATIRIMLARI</t>
-  </si>
-  <si>
-    <t>SLOT4</t>
-  </si>
-  <si>
-    <t>ESENYURTSPOR</t>
-  </si>
-  <si>
-    <t>SILIVRISPOR</t>
-  </si>
-  <si>
-    <t>2.GRUP</t>
-  </si>
-  <si>
-    <t>Dudullu Sahasi</t>
-  </si>
-  <si>
-    <t>WEDNESDAY</t>
-  </si>
-  <si>
-    <t>SARIYER YENIMAHALLESPOR</t>
-  </si>
-  <si>
-    <t>ALIBEYKOYSPOR</t>
-  </si>
-  <si>
-    <t>Silivri Sahasi</t>
-  </si>
-  <si>
-    <t>TUESDAY</t>
-  </si>
-  <si>
-    <t>CAFERAGASPOR</t>
-  </si>
-  <si>
-    <t>YENIKOYSPOR</t>
-  </si>
-  <si>
-    <t>SLOT1</t>
-  </si>
-  <si>
-    <t>BEYOGLUSPOR</t>
-  </si>
-  <si>
-    <t>CIBALISPOR</t>
-  </si>
-  <si>
     <t>CADDEBOSTANSPOR</t>
   </si>
   <si>
     <t>SULTANAHMETSPOR</t>
-  </si>
-  <si>
-    <t>MALTEPESPOR</t>
-  </si>
-  <si>
-    <t>KARTAL SPORTIF FAALIYETLERI</t>
-  </si>
-  <si>
-    <t>Beykoz Sahasi</t>
-  </si>
-  <si>
-    <t>MONDAY</t>
-  </si>
-  <si>
-    <t>BEYKOZ ISHAKLI SPOR FAALIYETLERI</t>
-  </si>
-  <si>
-    <t>ISTANBUL BEYLIKDUZUSPOR</t>
-  </si>
-  <si>
-    <t>HALICSPOR</t>
-  </si>
-  <si>
-    <t>VEFASPOR</t>
-  </si>
-  <si>
-    <t>INKILAP FUTBOL SPOR KULUBU</t>
-  </si>
-  <si>
-    <t>BAYRAMPASA SPOR</t>
-  </si>
-  <si>
-    <t>Seyrantepe Sahasi</t>
-  </si>
-  <si>
-    <t>BEYLERBEYI 1911 FUTBOL KULUBU</t>
-  </si>
-  <si>
-    <t>KUCUKCEKMECE SPORTIF FAALIYETLERI</t>
-  </si>
-  <si>
-    <t>FATIH KARAGUMRUK SPOR</t>
-  </si>
-  <si>
-    <t>BAHCESEHIRSPOR</t>
-  </si>
-  <si>
-    <t>ABBASAGASPOR</t>
-  </si>
-  <si>
-    <t>EYUPSULTANSPOR</t>
-  </si>
-  <si>
-    <t>ESENLERSPOR</t>
-  </si>
-  <si>
-    <t>KARTALSPOR</t>
-  </si>
-  <si>
-    <t>FERIKOYSPOR</t>
-  </si>
-  <si>
-    <t>KADIKOYSPOR</t>
-  </si>
-  <si>
-    <t>GUNGORENSPOR</t>
-  </si>
-  <si>
-    <t>BAKIRKOYSPOR</t>
-  </si>
-  <si>
-    <t>GAZIOSMANPASASPOR</t>
-  </si>
-  <si>
-    <t>SARIYERSPOR</t>
-  </si>
-  <si>
-    <t>TAKSIMSPOR</t>
-  </si>
-  <si>
-    <t>BAGCILARSPOR</t>
-  </si>
-  <si>
-    <t>FLORYASPOR</t>
-  </si>
-  <si>
-    <t>KABATASSPOR</t>
-  </si>
-  <si>
-    <t>SERENCEBEYSPOR</t>
-  </si>
-  <si>
-    <t>TUZLASPOR</t>
   </si>
 </sst>
 </file>
@@ -776,7 +776,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -796,7 +796,7 @@
         <v>12</v>
       </c>
       <c r="G2" s="7">
-        <v>45270</v>
+        <v>45264</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
@@ -810,39 +810,39 @@
         <v>9</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G3" s="7">
-        <v>45269</v>
+        <v>45264</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G4" s="7">
-        <v>45269</v>
+        <v>45265</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
@@ -853,177 +853,177 @@
         <v>21</v>
       </c>
       <c r="C5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="E5" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G5" s="7">
-        <v>45267</v>
+        <v>45264</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="E6" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="G6" s="7">
-        <v>45267</v>
+        <v>45264</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="F7" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G7" s="7">
-        <v>45266</v>
+        <v>45267</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>35</v>
-      </c>
       <c r="E8" s="4" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G8" s="7">
-        <v>45265</v>
+        <v>45264</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="7">
+        <v>45267</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
+      <c r="A10" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="B10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="C10" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="7">
+        <v>45264</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="A11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G9" s="7">
-        <v>45265</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="4" t="s">
+      <c r="C11" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="G11" s="7">
+        <v>45264</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+      <c r="A12" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" s="7">
-        <v>45265</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
-      <c r="A11" s="4" t="s">
+      <c r="B12" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C12" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="7">
-        <v>45265</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
-      <c r="A12" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="G12" s="7">
         <v>45264</v>
@@ -1031,22 +1031,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="G13" s="7">
         <v>45264</v>
@@ -1054,45 +1054,45 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C14" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>31</v>
-      </c>
       <c r="E14" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="G14" s="7">
-        <v>45264</v>
+        <v>45266</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C15" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>54</v>
-      </c>
       <c r="E15" s="4" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="G15" s="7">
         <v>45264</v>
@@ -1100,45 +1100,45 @@
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="G16" s="7">
         <v>45264</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G17" s="7">
         <v>45264</v>
@@ -1146,22 +1146,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="G18" s="7">
         <v>45264</v>
@@ -1169,22 +1169,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="G19" s="7">
         <v>45264</v>
@@ -1192,71 +1192,71 @@
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>47</v>
-      </c>
       <c r="F20" s="4" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="G20" s="7">
-        <v>45264</v>
+        <v>45270</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>66</v>
-      </c>
       <c r="C21" s="13" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>12</v>
       </c>
       <c r="G21" s="7">
-        <v>45264</v>
+        <v>45265</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="C22" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G22" s="7">
-        <v>45264</v>
+        <v>45269</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
@@ -1267,19 +1267,19 @@
         <v>70</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="G23" s="7">
-        <v>45264</v>
+        <v>45265</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
@@ -1290,22 +1290,22 @@
         <v>72</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="G24" s="7">
-        <v>45264</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
+        <v>45269</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="20.25">
       <c r="A25" s="4" t="s">
         <v>73</v>
       </c>
@@ -1313,19 +1313,19 @@
         <v>74</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="G25" s="7">
-        <v>45264</v>
+        <v>45265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>